<commit_message>
add xlsx_Extractor - it's work, but need vremyapartii
</commit_message>
<xml_diff>
--- a/Реестр_2021-09-08.xlsx
+++ b/Реестр_2021-09-08.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+  <si>
+    <t>№ п/п</t>
+  </si>
   <si>
     <t>Децимальный №</t>
   </si>
@@ -22,6 +25,12 @@
     <t>Наименование</t>
   </si>
   <si>
+    <t>Площадь поверхности, мм2</t>
+  </si>
+  <si>
+    <t>Глубина обработки, мм"</t>
+  </si>
+  <si>
     <t>Трудоемкость, н/ч</t>
   </si>
   <si>
@@ -31,37 +40,55 @@
     <t>Срок изготовления партии,  дней</t>
   </si>
   <si>
-    <t>rgrty4557</t>
-  </si>
-  <si>
-    <t>shina</t>
-  </si>
-  <si>
-    <t>Gas245</t>
-  </si>
-  <si>
-    <t>opora</t>
-  </si>
-  <si>
-    <t>Fo345od</t>
-  </si>
-  <si>
-    <t>Palka</t>
-  </si>
-  <si>
-    <t>G13ym</t>
-  </si>
-  <si>
-    <t>srert</t>
-  </si>
-  <si>
-    <t>er45od</t>
-  </si>
-  <si>
-    <t>Pachka</t>
-  </si>
-  <si>
-    <t>Hello</t>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>trt574</t>
+  </si>
+  <si>
+    <t>grfdgh</t>
+  </si>
+  <si>
+    <t>уеуке4еу4</t>
+  </si>
+  <si>
+    <t>пролд</t>
+  </si>
+  <si>
+    <t>цке57ук</t>
+  </si>
+  <si>
+    <t>опроа</t>
+  </si>
+  <si>
+    <t>ыв345й</t>
+  </si>
+  <si>
+    <t>вишня</t>
+  </si>
+  <si>
+    <t>dt4</t>
+  </si>
+  <si>
+    <t>sgdh</t>
+  </si>
+  <si>
+    <t>90fgt6</t>
+  </si>
+  <si>
+    <t>6hbdct</t>
+  </si>
+  <si>
+    <t>цукк356к</t>
+  </si>
+  <si>
+    <t>лопата</t>
+  </si>
+  <si>
+    <t>веп353</t>
+  </si>
+  <si>
+    <t>ааыа</t>
   </si>
 </sst>
 </file>
@@ -402,13 +429,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,115 +451,221 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>56</v>
+      </c>
+      <c r="E2">
+        <v>345</v>
+      </c>
+      <c r="F2">
+        <v>9.66</v>
+      </c>
+      <c r="G2">
+        <v>22701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>46778</v>
+      </c>
+      <c r="E3">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>1309.784</v>
+      </c>
+      <c r="G3">
+        <v>3077992.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>457</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0.6855</v>
+      </c>
+      <c r="G4">
+        <v>1610.925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>23.55</v>
-      </c>
-      <c r="D2">
-        <v>245.6</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>2.54</v>
-      </c>
-      <c r="D3">
-        <v>300.54</v>
-      </c>
-      <c r="E3">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>1.234</v>
-      </c>
-      <c r="D4">
-        <v>23535</v>
-      </c>
-      <c r="E4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>45.36</v>
+        <v>345</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>13</v>
+      <c r="F5">
+        <v>1.035</v>
+      </c>
+      <c r="G5">
+        <v>2432.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>1.2</v>
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>354</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>15</v>
+      <c r="F6">
+        <v>0.354</v>
+      </c>
+      <c r="G6">
+        <v>831.9000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>568</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>1.988</v>
+      </c>
+      <c r="G7">
+        <v>4671.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>988</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>3.458</v>
+      </c>
+      <c r="G8">
+        <v>8126.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>466</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0.6990000000000001</v>
+      </c>
+      <c r="G9">
+        <v>1642.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>456</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="G10">
+        <v>1607.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add xlsx_Extractor - it's work
</commit_message>
<xml_diff>
--- a/Реестр_2021-09-08.xlsx
+++ b/Реестр_2021-09-08.xlsx
@@ -483,6 +483,9 @@
       <c r="G2">
         <v>22701</v>
       </c>
+      <c r="H2">
+        <v>457</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
@@ -506,6 +509,9 @@
       <c r="G3">
         <v>3077992.4</v>
       </c>
+      <c r="H3">
+        <v>456</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
@@ -529,6 +535,9 @@
       <c r="G4">
         <v>1610.925</v>
       </c>
+      <c r="H4">
+        <v>4380</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
@@ -552,6 +561,9 @@
       <c r="G5">
         <v>2432.25</v>
       </c>
+      <c r="H5">
+        <v>234</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
@@ -574,6 +586,9 @@
       </c>
       <c r="G6">
         <v>831.9000000000001</v>
+      </c>
+      <c r="H6">
+        <v>9875</v>
       </c>
     </row>
     <row r="7" spans="1:8">

</xml_diff>